<commit_message>
updated information, added surge hand, updated page format slightly
</commit_message>
<xml_diff>
--- a/data/HAND_RoboticHandResearch.xlsx
+++ b/data/HAND_RoboticHandResearch.xlsx
@@ -11,14 +11,93 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="P+bt4Bf+6tpr70GqTcUynAuAgp/fo2RhusOYXS1xsFk="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="ect6GYs/4JcH4kpwTJGga1OU2L5XjoMaadsnL3ZvSVc="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="G24">
+      <text>
+        <t xml:space="preserve">======
+ID#AAABwu1E8Xk
+Ryan Hay    (2025-11-25 19:00:07)
+I changed it from "Unspecified number and type of actuators" to "22 active DoF", let me know if I should change it back</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="G13">
+      <text>
+        <t xml:space="preserve">======
+ID#AAABwo6FCAs
+Shihan Lu    (2025-11-24 08:45:31)
+Where did you find the Bowden cable transmission info?
+------
+ID#AAABwu1ElAw
+Ryan Hay    (2025-11-25 18:43:25)
+I found it on this datasheet: https://www.prensilia.com/wp-content/uploads/2023/03/Prensilia_data-sheet-IH2-AZZURRA-Hand.pdf</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="G37">
+      <text>
+        <t xml:space="preserve">======
+ID#AAABwo6FCAE
+Shihan Lu    (2025-11-24 07:51:10)
+Where did you find the "Hollow cup and Multi-link mechanism"?
+------
+ID#AAABwu1ElAo
+Ryan Hay    (2025-11-25 18:39:38)
+I just switched it to coreless motor and multilink mechanism as it says at the bottom of this page: https://paxini.com/dex/gen3</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="G14">
+      <text>
+        <t xml:space="preserve">======
+ID#AAABwo6FB_8
+Shihan Lu    (2025-11-24 07:24:21)
+Where did you find the "Geneva mechanism drive" info?
+------
+ID#AAABwu1ElAs
+Ryan Hay    (2025-11-25 18:42:47)
+It says on page 8 of this user manual. It might be important to note that the user manual is from 2021. https://www.prensilia.com/wp-content/uploads/2021/06/210529_Mia_UserManual_web.pdf</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="G40">
+      <text>
+        <t xml:space="preserve">======
+ID#AAABwpZHFb0
+Shihan Lu    (2025-11-23 09:02:21)
+Where did you find this info?
+------
+ID#AAABwu1ElAk
+Ryan Hay    (2025-11-25 18:29:33)
+I found it in this video from Boston Dynamics (the link is timestamped) https://youtu.be/gS4rOqNDTBk?si=8Zeg7gsyP_tHOd_Y&amp;t=86</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="I17">
+      <text>
+        <t xml:space="preserve">======
+ID#AAABwpZHFbo
+Shihan Lu    (2025-11-23 08:29:19)
+Got it</t>
+      </text>
+    </comment>
+  </commentList>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mixKi92vdH9mmgezs/HTo97Femd0w=="/>
+    </ext>
+  </extLst>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="726">
   <si>
     <t>Hand</t>
   </si>
@@ -1814,22 +1893,19 @@
     <t>shadow-dexterous-hand.png</t>
   </si>
   <si>
-    <t>20 brushed DC motors. Tendon-driven. Shadow Tactile Sensing (STF) with magnets and 3-axis Hall effect sensors on index and thumb (default). Motors stored in the hand base; tendons prone to wear with extensive use. Full ROS integration.</t>
+    <t>20 geared brushed DC motors pulling tendons passing through Bowden tubes at wrist. Each finger has 3 independently driven DOF and a fourth coupled DOF. Option to reduce from 4 fingers and a thumb to 3, 2, or 1 fingers and a thumb. 1-DOF palm flex. Wrist: 2 DOF. Communication: EtherCAT. Optional fingertip tactile sensors.</t>
   </si>
   <si>
     <t>Nov 2025</t>
   </si>
   <si>
-    <t>Given that we have it, is it backdrivable?</t>
-  </si>
-  <si>
     <t>https://www.shadowrobot.com/dex-ee/</t>
   </si>
   <si>
     <t>shadow_dex_ee.jpg</t>
   </si>
   <si>
-    <t>15 DC motors. Tendon-driven. Distal tactile sensors (magnets and 3-axis Hall effect) with optional middle and proximal sensors. Modular finger and sensor design; motors stored in finger bases. Backdrivable. Full ROS integration.</t>
+    <t xml:space="preserve">15 DC motors. Tendon-driven transmission: each finger has five motors driving four joints to reduce backlash and ensure smooth force/torque control (e.g., N+1 tendon routing). Distributed taxel arrays along the finger segments with vision-based tactile sensing in the fingertips. Modular finger and sensor design; motors stored in finger bases. Full ROS integration. Built to endure long-running, physically demanding experiments, including impacts and collisions. </t>
   </si>
   <si>
     <t>https://www.robotera.com/en/goods1/4.html</t>
@@ -1838,7 +1914,7 @@
     <t>xhand1.png</t>
   </si>
   <si>
-    <t>12 motors. Quasi-Direct Drive (QDD). Tactile arrays (&gt;100 points) on each finger. Thumb can be repositioned to pinky location for enhanced grip. Backdrivable. Supports Linux, SDK, and ROS.</t>
+    <t>12 motors. Quasi-Direct Drive (QDD). Tactile arrays (&gt;100 points) on each finger. Thumb can be repositioned to pinky location for enhanced grip. Supports Linux, SDK, and ROS.</t>
   </si>
   <si>
     <t>https://www.allegrohand.com/v5-4fplus</t>
@@ -1859,6 +1935,21 @@
     <t>16 DC motors. Gear-driven. No built-in tactile sensing. Widely used for dexterity research. Supports Linux, Windows, and ROS.</t>
   </si>
   <si>
+    <t>Alt-Bionics</t>
+  </si>
+  <si>
+    <t>https://www.altbionics.com/robotics/</t>
+  </si>
+  <si>
+    <t>surgehand.png</t>
+  </si>
+  <si>
+    <t>6 active DoF. Gear-driven. Optional advanced force sensors coming soon. Fully modular fingers enabling quick repairs. Rubberized fingers and palmar surfaces. Supports RS485 and CAN communication.</t>
+  </si>
+  <si>
+    <t>Couldn't find number actuators or actuator type.</t>
+  </si>
+  <si>
     <t>https://schunk.com/us/en/gripping-systems/special-gripper/svh/c/PGR_3161</t>
   </si>
   <si>
@@ -1868,9 +1959,6 @@
     <t>9 DC motors. Gear-driven (and spindle drives). No built-in tactile sensing. Features elastic gripping surfaces; power and control electronics integrated in the wrist. Supports ROS and Raspberry Pi.</t>
   </si>
   <si>
-    <t>Mentions nine drive motors in the operating manual. The function page says there is a servo motor connected to a spindle.</t>
-  </si>
-  <si>
     <t>https://www.psyonic.io/robots</t>
   </si>
   <si>
@@ -1886,7 +1974,7 @@
     <t>prohand.png</t>
   </si>
   <si>
-    <t>Unspecified number and type of actuators. Tendon-driven. Tactile sensing (type unspecified). The specifications are not finalized; planned to release in 2028.</t>
+    <t>Unspecified number and type of actuators. Tendon-driven. Tactile sensing (type unspecified). The specifications are not finalized; planned to release in December, 2025.</t>
   </si>
   <si>
     <t>https://www.dmrobot.com/en/products/p2/dm-hand1.html</t>
@@ -1904,10 +1992,7 @@
     <t>covvirobotichand.png</t>
   </si>
   <si>
-    <t>6 actuators (unspecified). Gear-driven. Force Sensing Resistor (FSR) in all fingertips. The index finger is touchscreen compatible and features a serrated fingertip texture for improved grip. Adapted from COVVI Prosthetic Hand. Compatible with ROS2 and Python ECI API.</t>
-  </si>
-  <si>
-    <t>Actuator type not specified</t>
+    <t>6 actuators (unspecified). Gear-driven. Springs integrated in transmission. Force Sensing Resistor (FSR) in all fingertips. The index finger is touchscreen compatible and features a serrated fingertip texture for improved grip. Adapted from COVVI Prosthetic Hand. Compatible with ROS2 and Python ECI API.</t>
   </si>
   <si>
     <t>https://www.prensilia.com/ih2-azzurra-hand/</t>
@@ -1949,9 +2034,6 @@
     <t>2 DC motors. Tendon-driven. No built-in tactile sensing. Features dislocatable, self-healing finger joints and interchangeable gloves. Compatible with ROS and ROS2.</t>
   </si>
   <si>
-    <t>It does not specifically state tendon-driven but given that SoftHand is tendon driven, I have assumed tendon-driven</t>
-  </si>
-  <si>
     <t>https://en.tesollo.com/dg-5f/</t>
   </si>
   <si>
@@ -1970,7 +2052,7 @@
     <t>dg4f.png</t>
   </si>
   <si>
-    <t>Unspecified number of DC motors. Unspecified transmission type. Optional fingertip Force/Torque (F/T) sensors. Adaptive gripping capability: fingers can shift to form right hand, left hand, or gripper.</t>
+    <t>Unspecified number of DC motors. Optional fingertip Force/Torque (F/T) sensors. Adaptive gripping capability: fingers can shift to form right hand, left hand, or gripper.</t>
   </si>
   <si>
     <t>Unsure about number of actuators.</t>
@@ -1982,7 +2064,7 @@
     <t>dg3fm.png</t>
   </si>
   <si>
-    <t>Unspecified number of brushless DC motors. Unspecified transmission type. Optional fingertip Force/Torque (F/T) sensors. Features a fully modular structure. Supports C/C++ and an SDK.</t>
+    <t>Unspecified number of brushless DC motors. Optional fingertip Force/Torque (F/T) sensors. Improved mechanical robustness and control precision. Features a fully modular structure. Supports C/C++ and an SDK.</t>
   </si>
   <si>
     <t>https://en.tesollo.com/dg-3f-b/</t>
@@ -1991,7 +2073,7 @@
     <t>dg3fb.png</t>
   </si>
   <si>
-    <t>Unspecified number of brushless DC motors. Unspecified transmission type. No built-in tactile sensing. Offers optional suction-type fingertips.</t>
+    <t>Unspecified number of brushless DC motors. No built-in tactile sensing. Offers optional suction-type fingertips.</t>
   </si>
   <si>
     <t>https://www.seedrobotics.com/rh8d-adult-robot-hand</t>
@@ -2027,7 +2109,7 @@
     <t>Sharpa.png</t>
   </si>
   <si>
-    <t>Unspecified number and type of actuators. Unspecified transmission type. Dynamic Tactile Array (DTA) capable of detecting up to 30N. Lifespan of over 1 million grip cycles. Backdrivable. Supports ROS, Linux, C++, Python, and Windows.</t>
+    <t>22 active DoF. Unspecified transmission type. Dynamic Tactile Array (DTA) capable of detecting up to 30N. Lifespan of over 1 million grip cycles. Backdrivable. Supports ROS, Linux, C++, Python, and Windows. Expected release in 2026.</t>
   </si>
   <si>
     <t>The hand claims 22 active DoF</t>
@@ -2039,7 +2121,7 @@
     <t>Aidin.png</t>
   </si>
   <si>
-    <t>Unspecified number and type of actuators. Unspecified transmission type. 6-axis Force/Torque (F/T) sensors on each fingertip. For research use only.</t>
+    <t>Linkage-driven. 6-axis Force/Torque (F/T) sensors on each fingertip. For research use only.</t>
   </si>
   <si>
     <t>https://inspire-robots.store/collections/all/products/dexterous-hand-rh56dfx-series?variant=42723202072820</t>
@@ -2048,7 +2130,7 @@
     <t>DexterousHandsDFX.png</t>
   </si>
   <si>
-    <t>6 miniature linear servo actuators. Linear-drive. Integrated force and tactile sensors. Two variants: BFX (greater speed) and DFX (greater grip force). Supports ROS.</t>
+    <t>6 miniature linear servo actuators with 12 motorized joints. Linear-drive. Hybrid force and position control. Six integrated pressure sensors. Two variants: BFX (greater speed) and DFX (greater grip force). Supports ROS.</t>
   </si>
   <si>
     <t>The Dexterous Hands RH56DFTP</t>
@@ -2060,7 +2142,7 @@
     <t>DexterousHandsDFTP.png</t>
   </si>
   <si>
-    <t>6 miniature linear servo actuators. Linear-drive. 17 tactile sensors and 6 pressure sensors built-in. Fingertips can exert up to 3 kg.</t>
+    <t>6 miniature linear servo actuators with 12 motorized joints. Linear-drive. 17 tactile sensors and 6 pressure sensors built-in. Extended lifespan and mimics the size of human hands. Fingertips can exert a force of up to 3 kg.</t>
   </si>
   <si>
     <t>BarrettHand</t>
@@ -2072,7 +2154,7 @@
     <t>BarrettHand.png</t>
   </si>
   <si>
-    <t>4 brushless DC servo motors. Worm-drive and cable drive transmission. Optional torque and tactile sensing in fingertips; features a perception palm sensor that uses cameras, lasers, LED, and infrared to assist with object localization. Modular finger design.</t>
+    <t>4 brushless DC servo motors. Worm drives integrated with proprietary cable drive and breakaway clutch. Position sensing at each motor. Optional torque and tactile sensing in fingertips; features a perception palm sensor that uses cameras, lasers, LED, and infrared to assist with object localization. Modular finger design.</t>
   </si>
   <si>
     <t>https://www.hiwonder.com/products/uhandpi?variant=40961372618839</t>
@@ -2081,7 +2163,7 @@
     <t>uHandPi.png</t>
   </si>
   <si>
-    <t>6 servo motors. Linkage-driven. No built-in tactile sensing. Utilizes camera for AI image recognition, finger-guessing, etc. Integrated with Raspberry Pi 5.</t>
+    <t>6 servo motors. Linkage-driven. No built-in tactile sensing. Utilizes camera for AI image recognition, finger-guessing, etc. Integrated with Raspberry Pi 5. Super cheap hand; mainly for education.</t>
   </si>
   <si>
     <t>https://www.agile-robots.com/en/robotic-solutions/agile-hand</t>
@@ -2090,7 +2172,7 @@
     <t>agilehand.png</t>
   </si>
   <si>
-    <t>Unspecified number and type of actuators. Unspecified transmission type. Optional tactile sensing. Features a modular finger design and optional independent thumb actuator. Compatible with C++, Python, and ROS.</t>
+    <t>Unspecified number and type of actuators. Unspecified transmission type. Multisensory tactile sensing. Equipped with active compliant control strategies. Features a modular finger design and optional independent thumb actuator. Compatible with C++, Python, and ROS.</t>
   </si>
   <si>
     <t>https://www.figure.ai/</t>
@@ -2099,7 +2181,7 @@
     <t>f02hand.png</t>
   </si>
   <si>
-    <t>Unspecified number and type of actuators. Unspecified transmission type. Unspecified tactile sensing. Part of the Figure 02 humanoid robot.</t>
+    <t xml:space="preserve">Part of the Figure 02 humanoid robot. Details are unavailable. </t>
   </si>
   <si>
     <t>https://www.tesla.com/AI</t>
@@ -2108,16 +2190,7 @@
     <t>optimushand.png</t>
   </si>
   <si>
-    <t>Unspecified number and type of actuators. Unspecified transmission type. Unspecified tactile sensing. Part of the Optimus humanoid robot.</t>
-  </si>
-  <si>
-    <t>https://www.roboworks.net/store/p/smarthands</t>
-  </si>
-  <si>
-    <t>smarthands.png</t>
-  </si>
-  <si>
-    <t>6 micro linear servo motors. Linear-drive. 6 pressure sensors. Integrated with ROS (ROS2 Foxy).</t>
+    <t xml:space="preserve">Part of the Optimus humanoid robot. Details are unavailable. </t>
   </si>
   <si>
     <t>https://www.unitree.com/Dex5-1</t>
@@ -2126,10 +2199,7 @@
     <t>dex5-1p.png</t>
   </si>
   <si>
-    <t>Unspecified number of DC motors. Gear-driven. 94 tactile sensors in total. Backdrivable. Features a modular finger design.</t>
-  </si>
-  <si>
-    <t>16 active DoF, I have been assuming that does not necessarily mean 16 motors.</t>
+    <t>16 active and 4 passive DOF. Gear-driven. Fast reflex and high flexibility. Ultra-small joint gaps. 94 tactile sensors over fingertips, finger phalanges, and palm. Backdrivable. Features a modular finger design.</t>
   </si>
   <si>
     <t>https://www.unitree.com/Dex3-1</t>
@@ -2138,7 +2208,7 @@
     <t>dex3-1.png</t>
   </si>
   <si>
-    <t>7 micro brushless DC motors. 6 Direct-drive, 1 gear-driven. 33 tactile sensors on fingertips, finger phalanges, and palm. Compatible with Unitree G1 humanoid robot.</t>
+    <t>7 micro brushless DC motors - 6 direct-drive and 1 gear-drive. 33 tactile sensors on fingertips, finger phalanges, and palm. Communication: Unibus. Compatible with Unitree G1 humanoid robot.</t>
   </si>
   <si>
     <t>https://clonerobotics.com/hand</t>
@@ -2147,7 +2217,7 @@
     <t>clonehand.png</t>
   </si>
   <si>
-    <t>Artificial muscle fibers (Myofiber technology). Unspecified tactile sensing. Clone has not publicly disclosed detailed information on Myofiber.</t>
+    <t>Artificial muscle fibers (Myofiber technology). Extremely biomimetic. Clone has not publicly disclosed detailed information on Myofiber.</t>
   </si>
   <si>
     <t>https://daxo-robotics.com/</t>
@@ -2156,19 +2226,19 @@
     <t>musclev0.png</t>
   </si>
   <si>
-    <t>108 artificial muscle units. Unspecified number and type of actuators. Unspecified transmission type. Unspecified tactile sensing. Uses artificial muscles to achieve "infinite" degrees of freedom. A prototype.</t>
+    <t>108 artificial muscle units. Uses artificial muscles to achieve "infinite" degrees of freedom. AI powered to route power through other muscles in case of muscle failure. Continuum hand. A prototype.</t>
   </si>
   <si>
     <t>GMH18 GEN3</t>
   </si>
   <si>
-    <t>https://paxini.com/</t>
+    <t>https://paxini.com/dex/gen3</t>
   </si>
   <si>
     <t>gmh18.png</t>
   </si>
   <si>
-    <t>Unspecified number and type of actuators. Hollow cup and Multi-link mechanism. Over 1000 ITPU multi-dimensional tactile sensing units covering the fingernails, fingertips, finger pads, and palm; featuring 15 types of tactile perception. Supports camera expansion on the palm and back of hand.</t>
+    <t>11 active and 7 passive DOF. Coreless Motor and Multi-link mechanism. Proprietary force control algorithms and adaptive grasping based on object shape. ITPU multi-dimensional tactile sensing units covering the fingernails, fingertips, finger pads, and palm; capable of 15 types of tactile perception. Supports camera expansion on the palm and back of hand.</t>
   </si>
   <si>
     <t>https://oymotion.com/en/product62/191</t>
@@ -2177,7 +2247,7 @@
     <t>rohand.png</t>
   </si>
   <si>
-    <t>Unspecified number and type of actuators. Unspecified transmission type. No built-in tactile sensing. Used in inspection robots, prosthetics, and research. Supports SDK, ROS, and ROS2.</t>
+    <t>6 active and 5 passive DOF. No built-in tactile sensing. Lightweight and resembles the size and proportions of a human hand. Used in inspection robots, prosthetics, and research. Supports SDK, ROS, and ROS2.</t>
   </si>
   <si>
     <t>DexRobot</t>
@@ -2189,7 +2259,7 @@
     <t>dexrobot_hand.png</t>
   </si>
   <si>
-    <t>Unspecified number of motors. Tendon-driven. Equipped with position, force, and tactile sensors. Features independently replaceable fingers. Supports ROS and ROS2.</t>
+    <t>12 active and 7 passive DOF. Tendon-driven. Equipped with multimodal sensory feedback, including position, force, and tactile sensors. Features independently replaceable fingers. Supports ROS and ROS2.</t>
   </si>
   <si>
     <t>Atlas Gripper</t>
@@ -2204,7 +2274,7 @@
     <t>atlasgripper.png</t>
   </si>
   <si>
-    <t>7 actuators (type unspecified). Unspecified transmission type. Tactile sensors on fingertips and cameras in the palm. Feature an articulated thumb joint. Part of the Atlas humanoid robot.</t>
+    <t>7 actuators (type unspecified). Tactile sensors on fingertips and cameras in the palm. Feature an articulated thumb joint. Modular. Part of the Atlas humanoid robot.</t>
   </si>
 </sst>
 </file>
@@ -2357,7 +2427,7 @@
       <color rgb="FF0563C1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2388,6 +2458,18 @@
         <bgColor rgb="FFF9F9F9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6D7A8"/>
+        <bgColor rgb="FFB6D7A8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border/>
@@ -2401,7 +2483,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="121">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2636,7 +2718,7 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -2663,6 +2745,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2698,6 +2783,9 @@
     <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -2716,8 +2804,17 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -2729,6 +2826,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -26717,9 +26817,7 @@
       <c r="H2" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I2" s="84" t="s">
-        <v>600</v>
-      </c>
+      <c r="I2" s="84"/>
       <c r="J2" s="85"/>
       <c r="K2" s="6"/>
       <c r="L2" s="86"/>
@@ -26741,7 +26839,7 @@
         <v>18</v>
       </c>
       <c r="C3" s="89" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D3" s="80">
         <v>3.0</v>
@@ -26750,10 +26848,10 @@
         <v>15.0</v>
       </c>
       <c r="F3" s="81" t="s">
+        <v>601</v>
+      </c>
+      <c r="G3" s="82" t="s">
         <v>602</v>
-      </c>
-      <c r="G3" s="82" t="s">
-        <v>603</v>
       </c>
       <c r="H3" s="83" t="s">
         <v>599</v>
@@ -26780,7 +26878,7 @@
         <v>196</v>
       </c>
       <c r="C4" s="91" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D4" s="87">
         <v>5.0</v>
@@ -26789,21 +26887,21 @@
         <v>12.0</v>
       </c>
       <c r="F4" s="92" t="s">
+        <v>604</v>
+      </c>
+      <c r="G4" s="93" t="s">
         <v>605</v>
-      </c>
-      <c r="G4" s="81" t="s">
-        <v>606</v>
       </c>
       <c r="H4" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I4" s="93"/>
+      <c r="I4" s="94"/>
       <c r="J4" s="84"/>
-      <c r="K4" s="94"/>
+      <c r="K4" s="95"/>
       <c r="L4" s="86"/>
       <c r="M4" s="86"/>
       <c r="N4" s="86"/>
-      <c r="O4" s="95"/>
+      <c r="O4" s="96"/>
       <c r="P4" s="86"/>
       <c r="Q4" s="84"/>
       <c r="R4" s="84"/>
@@ -26812,14 +26910,14 @@
       <c r="U4" s="84"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="96" t="s">
+      <c r="A5" s="97" t="s">
         <v>438</v>
       </c>
       <c r="B5" s="78" t="s">
         <v>29</v>
       </c>
       <c r="C5" s="79" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D5" s="80">
         <v>4.0</v>
@@ -26828,17 +26926,17 @@
         <v>16.0</v>
       </c>
       <c r="F5" s="81" t="s">
+        <v>607</v>
+      </c>
+      <c r="G5" s="93" t="s">
         <v>608</v>
-      </c>
-      <c r="G5" s="81" t="s">
-        <v>609</v>
       </c>
       <c r="H5" s="83" t="s">
         <v>599</v>
       </c>
       <c r="I5" s="85"/>
       <c r="J5" s="84"/>
-      <c r="K5" s="94"/>
+      <c r="K5" s="95"/>
       <c r="L5" s="86"/>
       <c r="M5" s="86"/>
       <c r="N5" s="86"/>
@@ -26848,17 +26946,17 @@
       <c r="R5" s="84"/>
       <c r="S5" s="86"/>
       <c r="T5" s="84"/>
-      <c r="U5" s="97"/>
+      <c r="U5" s="98"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="96" t="s">
+      <c r="A6" s="97" t="s">
         <v>444</v>
       </c>
-      <c r="B6" s="96" t="s">
+      <c r="B6" s="97" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="79" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D6" s="90">
         <v>4.0</v>
@@ -26867,19 +26965,17 @@
         <v>16.0</v>
       </c>
       <c r="F6" s="81" t="s">
+        <v>610</v>
+      </c>
+      <c r="G6" s="93" t="s">
         <v>611</v>
-      </c>
-      <c r="G6" s="81" t="s">
-        <v>612</v>
       </c>
       <c r="H6" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I6" s="84" t="s">
-        <v>600</v>
-      </c>
+      <c r="I6" s="84"/>
       <c r="J6" s="84"/>
-      <c r="K6" s="94"/>
+      <c r="K6" s="95"/>
       <c r="L6" s="86"/>
       <c r="M6" s="86"/>
       <c r="N6" s="86"/>
@@ -26889,23 +26985,23 @@
       <c r="R6" s="84"/>
       <c r="S6" s="86"/>
       <c r="T6" s="84"/>
-      <c r="U6" s="97"/>
+      <c r="U6" s="98"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="96" t="s">
-        <v>449</v>
-      </c>
-      <c r="B7" s="78" t="s">
-        <v>73</v>
+      <c r="A7" s="97" t="s">
+        <v>170</v>
+      </c>
+      <c r="B7" s="97" t="s">
+        <v>612</v>
       </c>
       <c r="C7" s="79" t="s">
         <v>613</v>
       </c>
-      <c r="D7" s="87">
+      <c r="D7" s="90">
         <v>5.0</v>
       </c>
-      <c r="E7" s="81">
-        <v>9.0</v>
+      <c r="E7" s="81" t="s">
+        <v>54</v>
       </c>
       <c r="F7" s="81" t="s">
         <v>614</v>
@@ -26920,7 +27016,7 @@
         <v>616</v>
       </c>
       <c r="J7" s="84"/>
-      <c r="K7" s="94"/>
+      <c r="K7" s="95"/>
       <c r="L7" s="86"/>
       <c r="M7" s="86"/>
       <c r="N7" s="14"/>
@@ -26930,14 +27026,14 @@
       <c r="R7" s="84"/>
       <c r="S7" s="86"/>
       <c r="T7" s="84"/>
-      <c r="U7" s="97"/>
+      <c r="U7" s="98"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="98" t="s">
-        <v>207</v>
+      <c r="A8" s="97" t="s">
+        <v>449</v>
       </c>
       <c r="B8" s="78" t="s">
-        <v>208</v>
+        <v>73</v>
       </c>
       <c r="C8" s="79" t="s">
         <v>617</v>
@@ -26945,640 +27041,634 @@
       <c r="D8" s="87">
         <v>5.0</v>
       </c>
-      <c r="E8" s="92">
-        <v>6.0</v>
-      </c>
-      <c r="F8" s="92" t="s">
+      <c r="E8" s="81">
+        <v>9.0</v>
+      </c>
+      <c r="F8" s="81" t="s">
         <v>618</v>
       </c>
-      <c r="G8" s="81" t="s">
+      <c r="G8" s="93" t="s">
         <v>619</v>
       </c>
       <c r="H8" s="83" t="s">
         <v>599</v>
       </c>
       <c r="I8" s="84"/>
-      <c r="J8" s="93"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="93"/>
-      <c r="M8" s="93"/>
-      <c r="N8" s="99"/>
-      <c r="O8" s="87"/>
+      <c r="J8" s="84"/>
+      <c r="K8" s="95"/>
+      <c r="L8" s="86"/>
+      <c r="M8" s="86"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="90"/>
       <c r="P8" s="86"/>
       <c r="Q8" s="84"/>
-      <c r="R8" s="93"/>
+      <c r="R8" s="84"/>
       <c r="S8" s="86"/>
       <c r="T8" s="84"/>
-      <c r="U8" s="84"/>
+      <c r="U8" s="98"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="96" t="s">
-        <v>469</v>
-      </c>
-      <c r="B9" s="100" t="s">
-        <v>470</v>
+      <c r="A9" s="99" t="s">
+        <v>207</v>
+      </c>
+      <c r="B9" s="78" t="s">
+        <v>208</v>
       </c>
       <c r="C9" s="79" t="s">
         <v>620</v>
       </c>
-      <c r="D9" s="95">
+      <c r="D9" s="87">
         <v>5.0</v>
       </c>
-      <c r="E9" s="81" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="81" t="s">
+      <c r="E9" s="92">
+        <v>6.0</v>
+      </c>
+      <c r="F9" s="92" t="s">
         <v>621</v>
       </c>
-      <c r="G9" s="81" t="s">
+      <c r="G9" s="93" t="s">
         <v>622</v>
       </c>
       <c r="H9" s="83" t="s">
         <v>599</v>
       </c>
       <c r="I9" s="84"/>
-      <c r="J9" s="84"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="101"/>
-      <c r="M9" s="86"/>
-      <c r="N9" s="86"/>
-      <c r="O9" s="90"/>
+      <c r="J9" s="94"/>
+      <c r="K9" s="95"/>
+      <c r="L9" s="94"/>
+      <c r="M9" s="94"/>
+      <c r="N9" s="100"/>
+      <c r="O9" s="87"/>
       <c r="P9" s="86"/>
       <c r="Q9" s="84"/>
-      <c r="R9" s="84"/>
+      <c r="R9" s="94"/>
       <c r="S9" s="86"/>
       <c r="T9" s="84"/>
-      <c r="U9" s="102"/>
+      <c r="U9" s="84"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="78" t="s">
-        <v>199</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="C10" s="103" t="s">
+      <c r="A10" s="97" t="s">
+        <v>469</v>
+      </c>
+      <c r="B10" s="101" t="s">
+        <v>470</v>
+      </c>
+      <c r="C10" s="79" t="s">
         <v>623</v>
       </c>
-      <c r="D10" s="87">
+      <c r="D10" s="96">
         <v>5.0</v>
       </c>
-      <c r="E10" s="86">
-        <v>6.0</v>
-      </c>
-      <c r="F10" s="86" t="s">
+      <c r="E10" s="81" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="81" t="s">
         <v>624</v>
       </c>
-      <c r="G10" s="81" t="s">
+      <c r="G10" s="93" t="s">
         <v>625</v>
       </c>
       <c r="H10" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I10" s="93"/>
+      <c r="I10" s="84"/>
       <c r="J10" s="84"/>
-      <c r="K10" s="94"/>
-      <c r="L10" s="86"/>
+      <c r="K10" s="95"/>
+      <c r="L10" s="102"/>
       <c r="M10" s="86"/>
       <c r="N10" s="86"/>
-      <c r="O10" s="95"/>
-      <c r="P10" s="14"/>
+      <c r="O10" s="90"/>
+      <c r="P10" s="86"/>
       <c r="Q10" s="84"/>
       <c r="R10" s="84"/>
       <c r="S10" s="86"/>
       <c r="T10" s="84"/>
-      <c r="U10" s="84"/>
+      <c r="U10" s="103"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="98" t="s">
-        <v>480</v>
+      <c r="A11" s="78" t="s">
+        <v>199</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="C11" s="91" t="s">
+        <v>200</v>
+      </c>
+      <c r="C11" s="104" t="s">
         <v>626</v>
       </c>
       <c r="D11" s="87">
         <v>5.0</v>
       </c>
-      <c r="E11" s="92">
+      <c r="E11" s="86">
         <v>6.0</v>
       </c>
-      <c r="F11" s="92" t="s">
+      <c r="F11" s="86" t="s">
         <v>627</v>
       </c>
-      <c r="G11" s="81" t="s">
+      <c r="G11" s="93" t="s">
         <v>628</v>
       </c>
       <c r="H11" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I11" s="93" t="s">
-        <v>629</v>
-      </c>
+      <c r="I11" s="94"/>
       <c r="J11" s="84"/>
-      <c r="K11" s="94"/>
+      <c r="K11" s="95"/>
       <c r="L11" s="86"/>
       <c r="M11" s="86"/>
       <c r="N11" s="86"/>
-      <c r="O11" s="80"/>
-      <c r="P11" s="86"/>
+      <c r="O11" s="96"/>
+      <c r="P11" s="14"/>
       <c r="Q11" s="84"/>
       <c r="R11" s="84"/>
       <c r="S11" s="86"/>
       <c r="T11" s="84"/>
-      <c r="U11" s="97"/>
+      <c r="U11" s="84"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="78" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="78" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" s="79" t="s">
-        <v>630</v>
+      <c r="A12" s="99" t="s">
+        <v>480</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C12" s="91" t="s">
+        <v>629</v>
       </c>
       <c r="D12" s="87">
         <v>5.0</v>
       </c>
       <c r="E12" s="92">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="F12" s="92" t="s">
+        <v>630</v>
+      </c>
+      <c r="G12" s="93" t="s">
         <v>631</v>
-      </c>
-      <c r="G12" s="81" t="s">
-        <v>632</v>
       </c>
       <c r="H12" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I12" s="84"/>
-      <c r="J12" s="85"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="104"/>
-      <c r="M12" s="104"/>
-      <c r="N12" s="104"/>
-      <c r="O12" s="87"/>
+      <c r="I12" s="94"/>
+      <c r="J12" s="84"/>
+      <c r="K12" s="95"/>
+      <c r="L12" s="86"/>
+      <c r="M12" s="86"/>
+      <c r="N12" s="86"/>
+      <c r="O12" s="80"/>
       <c r="P12" s="86"/>
       <c r="Q12" s="84"/>
       <c r="R12" s="84"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="85"/>
-      <c r="U12" s="97"/>
+      <c r="S12" s="86"/>
+      <c r="T12" s="84"/>
+      <c r="U12" s="98"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="96" t="s">
-        <v>633</v>
-      </c>
-      <c r="B13" s="88" t="s">
+      <c r="A13" s="78" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="78" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="105" t="s">
-        <v>634</v>
+      <c r="C13" s="79" t="s">
+        <v>632</v>
       </c>
       <c r="D13" s="87">
         <v>5.0</v>
       </c>
       <c r="E13" s="92">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="F13" s="92" t="s">
-        <v>635</v>
-      </c>
-      <c r="G13" s="81" t="s">
-        <v>636</v>
+        <v>633</v>
+      </c>
+      <c r="G13" s="105" t="s">
+        <v>634</v>
       </c>
       <c r="H13" s="83" t="s">
         <v>599</v>
       </c>
       <c r="I13" s="84"/>
       <c r="J13" s="85"/>
-      <c r="K13" s="94"/>
-      <c r="L13" s="86"/>
-      <c r="M13" s="86"/>
-      <c r="N13" s="86"/>
-      <c r="O13" s="90"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="106"/>
+      <c r="M13" s="106"/>
+      <c r="N13" s="106"/>
+      <c r="O13" s="87"/>
       <c r="P13" s="86"/>
       <c r="Q13" s="84"/>
-      <c r="R13" s="85"/>
+      <c r="R13" s="84"/>
       <c r="S13" s="14"/>
-      <c r="T13" s="84"/>
-      <c r="U13" s="97"/>
+      <c r="T13" s="85"/>
+      <c r="U13" s="98"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="98" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" s="78" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="79" t="s">
+      <c r="A14" s="97" t="s">
+        <v>635</v>
+      </c>
+      <c r="B14" s="88" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="107" t="s">
+        <v>636</v>
+      </c>
+      <c r="D14" s="87">
+        <v>5.0</v>
+      </c>
+      <c r="E14" s="92">
+        <v>3.0</v>
+      </c>
+      <c r="F14" s="92" t="s">
         <v>637</v>
       </c>
-      <c r="D14" s="80">
-        <v>5.0</v>
-      </c>
-      <c r="E14" s="92">
-        <v>1.0</v>
-      </c>
-      <c r="F14" s="92" t="s">
+      <c r="G14" s="105" t="s">
         <v>638</v>
-      </c>
-      <c r="G14" s="81" t="s">
-        <v>639</v>
       </c>
       <c r="H14" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I14" s="85"/>
-      <c r="J14" s="106"/>
-      <c r="K14" s="6"/>
+      <c r="I14" s="84"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="95"/>
       <c r="L14" s="86"/>
       <c r="M14" s="86"/>
       <c r="N14" s="86"/>
       <c r="O14" s="90"/>
-      <c r="P14" s="102"/>
-      <c r="Q14" s="85"/>
-      <c r="R14" s="93"/>
-      <c r="S14" s="86"/>
+      <c r="P14" s="86"/>
+      <c r="Q14" s="84"/>
+      <c r="R14" s="85"/>
+      <c r="S14" s="14"/>
       <c r="T14" s="84"/>
-      <c r="U14" s="97"/>
+      <c r="U14" s="98"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="96" t="s">
-        <v>501</v>
-      </c>
-      <c r="B15" s="88" t="s">
+      <c r="A15" s="99" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="78" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="89" t="s">
+      <c r="C15" s="79" t="s">
+        <v>639</v>
+      </c>
+      <c r="D15" s="80">
+        <v>5.0</v>
+      </c>
+      <c r="E15" s="92">
+        <v>1.0</v>
+      </c>
+      <c r="F15" s="92" t="s">
         <v>640</v>
       </c>
-      <c r="D15" s="87">
-        <v>5.0</v>
-      </c>
-      <c r="E15" s="81">
-        <v>2.0</v>
-      </c>
-      <c r="F15" s="81" t="s">
+      <c r="G15" s="93" t="s">
         <v>641</v>
-      </c>
-      <c r="G15" s="81" t="s">
-        <v>642</v>
       </c>
       <c r="H15" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I15" s="84" t="s">
-        <v>643</v>
-      </c>
-      <c r="J15" s="106"/>
+      <c r="I15" s="85"/>
+      <c r="J15" s="108"/>
       <c r="K15" s="6"/>
-      <c r="L15" s="92"/>
-      <c r="M15" s="92"/>
-      <c r="N15" s="104"/>
-      <c r="O15" s="87"/>
-      <c r="P15" s="86"/>
+      <c r="L15" s="86"/>
+      <c r="M15" s="86"/>
+      <c r="N15" s="86"/>
+      <c r="O15" s="90"/>
+      <c r="P15" s="103"/>
       <c r="Q15" s="85"/>
-      <c r="R15" s="93"/>
+      <c r="R15" s="94"/>
       <c r="S15" s="86"/>
       <c r="T15" s="84"/>
-      <c r="U15" s="97"/>
-    </row>
-    <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="107" t="s">
-        <v>130</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="C16" s="103" t="s">
-        <v>644</v>
+      <c r="U15" s="98"/>
+    </row>
+    <row r="16" ht="44.25" customHeight="1">
+      <c r="A16" s="97" t="s">
+        <v>501</v>
+      </c>
+      <c r="B16" s="88" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="89" t="s">
+        <v>642</v>
       </c>
       <c r="D16" s="87">
         <v>5.0</v>
       </c>
-      <c r="E16" s="92">
-        <v>20.0</v>
-      </c>
-      <c r="F16" s="92" t="s">
-        <v>645</v>
-      </c>
-      <c r="G16" s="81" t="s">
-        <v>646</v>
+      <c r="E16" s="81">
+        <v>2.0</v>
+      </c>
+      <c r="F16" s="81" t="s">
+        <v>643</v>
+      </c>
+      <c r="G16" s="93" t="s">
+        <v>644</v>
       </c>
       <c r="H16" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I16" s="84" t="s">
-        <v>647</v>
-      </c>
-      <c r="J16" s="94"/>
-      <c r="K16" s="94"/>
-      <c r="L16" s="93"/>
-      <c r="M16" s="93"/>
-      <c r="N16" s="93"/>
+      <c r="I16" s="84"/>
+      <c r="J16" s="108"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="92"/>
+      <c r="M16" s="92"/>
+      <c r="N16" s="106"/>
       <c r="O16" s="87"/>
-      <c r="P16" s="94"/>
+      <c r="P16" s="86"/>
       <c r="Q16" s="85"/>
       <c r="R16" s="94"/>
       <c r="S16" s="86"/>
       <c r="T16" s="84"/>
-      <c r="U16" s="97"/>
-    </row>
-    <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="107" t="s">
-        <v>136</v>
+      <c r="U16" s="98"/>
+    </row>
+    <row r="17" ht="49.5" customHeight="1">
+      <c r="A17" s="109" t="s">
+        <v>130</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="C17" s="103" t="s">
-        <v>648</v>
+      <c r="C17" s="104" t="s">
+        <v>645</v>
       </c>
       <c r="D17" s="87">
-        <v>4.0</v>
-      </c>
-      <c r="E17" s="81" t="s">
-        <v>54</v>
+        <v>5.0</v>
+      </c>
+      <c r="E17" s="92">
+        <v>20.0</v>
       </c>
       <c r="F17" s="92" t="s">
-        <v>649</v>
-      </c>
-      <c r="G17" s="81" t="s">
-        <v>650</v>
+        <v>646</v>
+      </c>
+      <c r="G17" s="93" t="s">
+        <v>647</v>
       </c>
       <c r="H17" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I17" s="94" t="s">
-        <v>651</v>
-      </c>
-      <c r="J17" s="94"/>
-      <c r="K17" s="94"/>
-      <c r="L17" s="93"/>
+      <c r="I17" s="84" t="s">
+        <v>648</v>
+      </c>
+      <c r="J17" s="95"/>
+      <c r="K17" s="95"/>
+      <c r="L17" s="94"/>
       <c r="M17" s="94"/>
-      <c r="N17" s="93"/>
+      <c r="N17" s="94"/>
       <c r="O17" s="87"/>
-      <c r="P17" s="94"/>
+      <c r="P17" s="95"/>
       <c r="Q17" s="85"/>
-      <c r="R17" s="94"/>
+      <c r="R17" s="95"/>
       <c r="S17" s="86"/>
-      <c r="T17" s="85"/>
-      <c r="U17" s="97"/>
+      <c r="T17" s="84"/>
+      <c r="U17" s="98"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="107" t="s">
-        <v>139</v>
+      <c r="A18" s="109" t="s">
+        <v>136</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="C18" s="103" t="s">
-        <v>652</v>
+      <c r="C18" s="104" t="s">
+        <v>649</v>
       </c>
       <c r="D18" s="87">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="E18" s="81" t="s">
         <v>54</v>
       </c>
       <c r="F18" s="92" t="s">
-        <v>653</v>
-      </c>
-      <c r="G18" s="81" t="s">
-        <v>654</v>
+        <v>650</v>
+      </c>
+      <c r="G18" s="93" t="s">
+        <v>651</v>
       </c>
       <c r="H18" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I18" s="94" t="s">
-        <v>651</v>
-      </c>
-      <c r="J18" s="94"/>
-      <c r="K18" s="94"/>
-      <c r="L18" s="93"/>
-      <c r="M18" s="93"/>
-      <c r="N18" s="93"/>
+      <c r="I18" s="95" t="s">
+        <v>652</v>
+      </c>
+      <c r="J18" s="95"/>
+      <c r="K18" s="95"/>
+      <c r="L18" s="94"/>
+      <c r="M18" s="95"/>
+      <c r="N18" s="94"/>
       <c r="O18" s="87"/>
-      <c r="P18" s="93"/>
+      <c r="P18" s="95"/>
       <c r="Q18" s="85"/>
-      <c r="R18" s="94"/>
+      <c r="R18" s="95"/>
       <c r="S18" s="86"/>
-      <c r="T18" s="84"/>
-      <c r="U18" s="97"/>
+      <c r="T18" s="85"/>
+      <c r="U18" s="98"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="98" t="s">
-        <v>142</v>
+      <c r="A19" s="109" t="s">
+        <v>139</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="C19" s="103" t="s">
-        <v>655</v>
-      </c>
-      <c r="D19" s="90">
+      <c r="C19" s="104" t="s">
+        <v>653</v>
+      </c>
+      <c r="D19" s="87">
         <v>3.0</v>
       </c>
       <c r="E19" s="81" t="s">
         <v>54</v>
       </c>
       <c r="F19" s="92" t="s">
-        <v>656</v>
-      </c>
-      <c r="G19" s="81" t="s">
-        <v>657</v>
+        <v>654</v>
+      </c>
+      <c r="G19" s="93" t="s">
+        <v>655</v>
       </c>
       <c r="H19" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I19" s="94" t="s">
-        <v>651</v>
-      </c>
-      <c r="J19" s="84"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="86"/>
+      <c r="I19" s="95" t="s">
+        <v>652</v>
+      </c>
+      <c r="J19" s="95"/>
+      <c r="K19" s="95"/>
+      <c r="L19" s="94"/>
       <c r="M19" s="94"/>
-      <c r="N19" s="86"/>
-      <c r="O19" s="80"/>
-      <c r="P19" s="93"/>
-      <c r="Q19" s="84"/>
-      <c r="R19" s="84"/>
-      <c r="S19" s="94"/>
+      <c r="N19" s="94"/>
+      <c r="O19" s="87"/>
+      <c r="P19" s="94"/>
+      <c r="Q19" s="85"/>
+      <c r="R19" s="95"/>
+      <c r="S19" s="86"/>
       <c r="T19" s="84"/>
-      <c r="U19" s="97"/>
+      <c r="U19" s="98"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="107" t="s">
-        <v>190</v>
+      <c r="A20" s="99" t="s">
+        <v>142</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="C20" s="103" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="104" t="s">
+        <v>656</v>
+      </c>
+      <c r="D20" s="90">
+        <v>3.0</v>
+      </c>
+      <c r="E20" s="81" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="92" t="s">
+        <v>657</v>
+      </c>
+      <c r="G20" s="93" t="s">
         <v>658</v>
-      </c>
-      <c r="D20" s="87">
-        <v>5.0</v>
-      </c>
-      <c r="E20" s="92">
-        <v>8.0</v>
-      </c>
-      <c r="F20" s="92" t="s">
-        <v>659</v>
-      </c>
-      <c r="G20" s="81" t="s">
-        <v>660</v>
       </c>
       <c r="H20" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I20" s="94"/>
+      <c r="I20" s="95" t="s">
+        <v>652</v>
+      </c>
       <c r="J20" s="84"/>
       <c r="K20" s="6"/>
       <c r="L20" s="86"/>
-      <c r="M20" s="94"/>
+      <c r="M20" s="95"/>
       <c r="N20" s="86"/>
       <c r="O20" s="80"/>
-      <c r="P20" s="93"/>
+      <c r="P20" s="94"/>
       <c r="Q20" s="84"/>
       <c r="R20" s="84"/>
-      <c r="S20" s="94"/>
+      <c r="S20" s="95"/>
       <c r="T20" s="84"/>
-      <c r="U20" s="97"/>
+      <c r="U20" s="98"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="96" t="s">
-        <v>523</v>
-      </c>
-      <c r="B21" s="108" t="s">
+      <c r="A21" s="109" t="s">
+        <v>190</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="C21" s="103" t="s">
+      <c r="C21" s="104" t="s">
+        <v>659</v>
+      </c>
+      <c r="D21" s="87">
+        <v>5.0</v>
+      </c>
+      <c r="E21" s="92">
+        <v>8.0</v>
+      </c>
+      <c r="F21" s="92" t="s">
+        <v>660</v>
+      </c>
+      <c r="G21" s="93" t="s">
         <v>661</v>
-      </c>
-      <c r="D21" s="95">
-        <v>4.0</v>
-      </c>
-      <c r="E21" s="81">
-        <v>6.0</v>
-      </c>
-      <c r="F21" s="81" t="s">
-        <v>662</v>
-      </c>
-      <c r="G21" s="81" t="s">
-        <v>663</v>
       </c>
       <c r="H21" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I21" s="94"/>
+      <c r="I21" s="95"/>
       <c r="J21" s="84"/>
       <c r="K21" s="6"/>
       <c r="L21" s="86"/>
-      <c r="M21" s="94"/>
+      <c r="M21" s="95"/>
       <c r="N21" s="86"/>
-      <c r="O21" s="90"/>
-      <c r="P21" s="93"/>
+      <c r="O21" s="80"/>
+      <c r="P21" s="94"/>
       <c r="Q21" s="84"/>
       <c r="R21" s="84"/>
-      <c r="S21" s="86"/>
+      <c r="S21" s="95"/>
       <c r="T21" s="84"/>
-      <c r="U21" s="97"/>
+      <c r="U21" s="98"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="96" t="s">
-        <v>527</v>
-      </c>
-      <c r="B22" s="108" t="s">
+      <c r="A22" s="97" t="s">
+        <v>523</v>
+      </c>
+      <c r="B22" s="110" t="s">
         <v>191</v>
       </c>
-      <c r="C22" s="103" t="s">
+      <c r="C22" s="104" t="s">
+        <v>662</v>
+      </c>
+      <c r="D22" s="96">
+        <v>4.0</v>
+      </c>
+      <c r="E22" s="81">
+        <v>6.0</v>
+      </c>
+      <c r="F22" s="81" t="s">
+        <v>663</v>
+      </c>
+      <c r="G22" s="93" t="s">
         <v>664</v>
-      </c>
-      <c r="D22" s="95">
-        <v>3.0</v>
-      </c>
-      <c r="E22" s="81">
-        <v>4.0</v>
-      </c>
-      <c r="F22" s="81" t="s">
-        <v>665</v>
-      </c>
-      <c r="G22" s="81" t="s">
-        <v>666</v>
       </c>
       <c r="H22" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I22" s="94"/>
+      <c r="I22" s="95"/>
       <c r="J22" s="84"/>
-      <c r="K22" s="94"/>
+      <c r="K22" s="6"/>
       <c r="L22" s="86"/>
-      <c r="M22" s="94"/>
+      <c r="M22" s="95"/>
       <c r="N22" s="86"/>
       <c r="O22" s="90"/>
-      <c r="P22" s="93"/>
+      <c r="P22" s="94"/>
       <c r="Q22" s="84"/>
       <c r="R22" s="84"/>
       <c r="S22" s="86"/>
       <c r="T22" s="84"/>
-      <c r="U22" s="97"/>
+      <c r="U22" s="98"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="107" t="s">
-        <v>165</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="C23" s="103" t="s">
+      <c r="A23" s="97" t="s">
+        <v>527</v>
+      </c>
+      <c r="B23" s="110" t="s">
+        <v>191</v>
+      </c>
+      <c r="C23" s="104" t="s">
+        <v>665</v>
+      </c>
+      <c r="D23" s="96">
+        <v>3.0</v>
+      </c>
+      <c r="E23" s="81">
+        <v>4.0</v>
+      </c>
+      <c r="F23" s="81" t="s">
+        <v>666</v>
+      </c>
+      <c r="G23" s="93" t="s">
         <v>667</v>
-      </c>
-      <c r="D23" s="87">
-        <v>5.0</v>
-      </c>
-      <c r="E23" s="81" t="s">
-        <v>54</v>
-      </c>
-      <c r="F23" s="84" t="s">
-        <v>668</v>
-      </c>
-      <c r="G23" s="81" t="s">
-        <v>669</v>
       </c>
       <c r="H23" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I23" s="86" t="s">
-        <v>670</v>
-      </c>
-      <c r="J23" s="86"/>
-      <c r="K23" s="86"/>
+      <c r="I23" s="95"/>
+      <c r="J23" s="84"/>
+      <c r="K23" s="95"/>
       <c r="L23" s="86"/>
-      <c r="M23" s="14"/>
+      <c r="M23" s="95"/>
       <c r="N23" s="86"/>
       <c r="O23" s="90"/>
-      <c r="P23" s="86"/>
+      <c r="P23" s="94"/>
       <c r="Q23" s="84"/>
-      <c r="R23" s="86"/>
+      <c r="R23" s="84"/>
       <c r="S23" s="86"/>
       <c r="T23" s="84"/>
-      <c r="U23" s="97"/>
+      <c r="U23" s="98"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="107" t="s">
-        <v>159</v>
+      <c r="A24" s="109" t="s">
+        <v>165</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="C24" s="103" t="s">
-        <v>671</v>
+        <v>166</v>
+      </c>
+      <c r="C24" s="104" t="s">
+        <v>668</v>
       </c>
       <c r="D24" s="87">
         <v>5.0</v>
@@ -27586,289 +27676,291 @@
       <c r="E24" s="81" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="92" t="s">
-        <v>672</v>
-      </c>
-      <c r="G24" s="81" t="s">
-        <v>673</v>
+      <c r="F24" s="84" t="s">
+        <v>669</v>
+      </c>
+      <c r="G24" s="105" t="s">
+        <v>670</v>
       </c>
       <c r="H24" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I24" s="86"/>
+      <c r="I24" s="86" t="s">
+        <v>671</v>
+      </c>
       <c r="J24" s="86"/>
       <c r="K24" s="86"/>
       <c r="L24" s="86"/>
       <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="87"/>
+      <c r="N24" s="86"/>
+      <c r="O24" s="90"/>
       <c r="P24" s="86"/>
-      <c r="Q24" s="86"/>
+      <c r="Q24" s="84"/>
       <c r="R24" s="86"/>
       <c r="S24" s="86"/>
-      <c r="T24" s="85"/>
-      <c r="U24" s="97"/>
+      <c r="T24" s="84"/>
+      <c r="U24" s="98"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="78" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" s="78" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="79" t="s">
+      <c r="A25" s="109" t="s">
+        <v>159</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C25" s="104" t="s">
+        <v>672</v>
+      </c>
+      <c r="D25" s="87">
+        <v>5.0</v>
+      </c>
+      <c r="E25" s="81" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" s="92" t="s">
+        <v>673</v>
+      </c>
+      <c r="G25" s="93" t="s">
         <v>674</v>
-      </c>
-      <c r="D25" s="80">
-        <v>5.0</v>
-      </c>
-      <c r="E25" s="86">
-        <v>6.0</v>
-      </c>
-      <c r="F25" s="86" t="s">
-        <v>675</v>
-      </c>
-      <c r="G25" s="81" t="s">
-        <v>676</v>
       </c>
       <c r="H25" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I25" s="85"/>
-      <c r="J25" s="85"/>
-      <c r="K25" s="6"/>
+      <c r="I25" s="86"/>
+      <c r="J25" s="86"/>
+      <c r="K25" s="86"/>
       <c r="L25" s="86"/>
-      <c r="M25" s="104"/>
-      <c r="N25" s="86"/>
-      <c r="O25" s="80"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="87"/>
       <c r="P25" s="86"/>
-      <c r="Q25" s="85"/>
+      <c r="Q25" s="86"/>
       <c r="R25" s="86"/>
-      <c r="S25" s="14"/>
+      <c r="S25" s="86"/>
       <c r="T25" s="85"/>
-      <c r="U25" s="97"/>
-    </row>
-    <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="96" t="s">
-        <v>677</v>
+      <c r="U25" s="98"/>
+    </row>
+    <row r="26" ht="61.5" customHeight="1">
+      <c r="A26" s="78" t="s">
+        <v>58</v>
       </c>
       <c r="B26" s="78" t="s">
         <v>59</v>
       </c>
       <c r="C26" s="79" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="D26" s="80">
         <v>5.0</v>
       </c>
-      <c r="E26" s="92">
+      <c r="E26" s="86">
         <v>6.0</v>
       </c>
       <c r="F26" s="86" t="s">
-        <v>679</v>
-      </c>
-      <c r="G26" s="81" t="s">
-        <v>680</v>
+        <v>676</v>
+      </c>
+      <c r="G26" s="93" t="s">
+        <v>677</v>
       </c>
       <c r="H26" s="83" t="s">
         <v>599</v>
       </c>
       <c r="I26" s="85"/>
       <c r="J26" s="85"/>
-      <c r="K26" s="86"/>
-      <c r="L26" s="104"/>
-      <c r="M26" s="109"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="86"/>
+      <c r="M26" s="106"/>
       <c r="N26" s="86"/>
       <c r="O26" s="80"/>
       <c r="P26" s="86"/>
-      <c r="Q26" s="84"/>
+      <c r="Q26" s="85"/>
       <c r="R26" s="86"/>
-      <c r="S26" s="86"/>
+      <c r="S26" s="14"/>
       <c r="T26" s="85"/>
-      <c r="U26" s="97"/>
-    </row>
-    <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="96" t="s">
+      <c r="U26" s="98"/>
+    </row>
+    <row r="27" ht="62.25" customHeight="1">
+      <c r="A27" s="97" t="s">
+        <v>678</v>
+      </c>
+      <c r="B27" s="78" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="79" t="s">
+        <v>679</v>
+      </c>
+      <c r="D27" s="80">
+        <v>5.0</v>
+      </c>
+      <c r="E27" s="92">
+        <v>6.0</v>
+      </c>
+      <c r="F27" s="86" t="s">
+        <v>680</v>
+      </c>
+      <c r="G27" s="93" t="s">
         <v>681</v>
-      </c>
-      <c r="B27" s="78" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="79" t="s">
-        <v>682</v>
-      </c>
-      <c r="D27" s="80">
-        <v>3.0</v>
-      </c>
-      <c r="E27" s="86">
-        <v>4.0</v>
-      </c>
-      <c r="F27" s="86" t="s">
-        <v>683</v>
-      </c>
-      <c r="G27" s="81" t="s">
-        <v>684</v>
       </c>
       <c r="H27" s="83" t="s">
         <v>599</v>
       </c>
       <c r="I27" s="85"/>
-      <c r="J27" s="86"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="86"/>
-      <c r="M27" s="86"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="87"/>
+      <c r="J27" s="85"/>
+      <c r="K27" s="86"/>
+      <c r="L27" s="106"/>
+      <c r="M27" s="111"/>
+      <c r="N27" s="86"/>
+      <c r="O27" s="80"/>
       <c r="P27" s="86"/>
-      <c r="Q27" s="85"/>
+      <c r="Q27" s="84"/>
       <c r="R27" s="86"/>
-      <c r="S27" s="14"/>
+      <c r="S27" s="86"/>
       <c r="T27" s="85"/>
-      <c r="U27" s="97"/>
+      <c r="U27" s="98"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="98" t="s">
-        <v>238</v>
-      </c>
-      <c r="B28" s="88" t="s">
-        <v>239</v>
-      </c>
-      <c r="C28" s="105" t="s">
+      <c r="A28" s="97" t="s">
+        <v>682</v>
+      </c>
+      <c r="B28" s="78" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="79" t="s">
+        <v>683</v>
+      </c>
+      <c r="D28" s="80">
+        <v>3.0</v>
+      </c>
+      <c r="E28" s="86">
+        <v>4.0</v>
+      </c>
+      <c r="F28" s="86" t="s">
+        <v>684</v>
+      </c>
+      <c r="G28" s="93" t="s">
         <v>685</v>
-      </c>
-      <c r="D28" s="80">
-        <v>5.0</v>
-      </c>
-      <c r="E28" s="92">
-        <v>6.0</v>
-      </c>
-      <c r="F28" s="92" t="s">
-        <v>686</v>
-      </c>
-      <c r="G28" s="84" t="s">
-        <v>687</v>
       </c>
       <c r="H28" s="83" t="s">
         <v>599</v>
       </c>
       <c r="I28" s="85"/>
-      <c r="J28" s="106"/>
+      <c r="J28" s="86"/>
       <c r="K28" s="6"/>
-      <c r="L28" s="93"/>
+      <c r="L28" s="86"/>
       <c r="M28" s="86"/>
-      <c r="N28" s="86"/>
+      <c r="N28" s="14"/>
       <c r="O28" s="87"/>
       <c r="P28" s="86"/>
-      <c r="Q28" s="84"/>
-      <c r="R28" s="85"/>
+      <c r="Q28" s="85"/>
+      <c r="R28" s="86"/>
       <c r="S28" s="14"/>
-      <c r="T28" s="84"/>
-      <c r="U28" s="97"/>
+      <c r="T28" s="85"/>
+      <c r="U28" s="98"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="78" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="78" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="79" t="s">
-        <v>688</v>
+      <c r="A29" s="99" t="s">
+        <v>238</v>
+      </c>
+      <c r="B29" s="88" t="s">
+        <v>239</v>
+      </c>
+      <c r="C29" s="107" t="s">
+        <v>686</v>
       </c>
       <c r="D29" s="80">
         <v>5.0</v>
       </c>
-      <c r="E29" s="81" t="s">
-        <v>54</v>
-      </c>
-      <c r="F29" s="81" t="s">
-        <v>689</v>
-      </c>
-      <c r="G29" s="84" t="s">
-        <v>690</v>
+      <c r="E29" s="92">
+        <v>6.0</v>
+      </c>
+      <c r="F29" s="92" t="s">
+        <v>687</v>
+      </c>
+      <c r="G29" s="112" t="s">
+        <v>688</v>
       </c>
       <c r="H29" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I29" s="86"/>
-      <c r="J29" s="86"/>
+      <c r="I29" s="85"/>
+      <c r="J29" s="108"/>
       <c r="K29" s="6"/>
-      <c r="L29" s="86"/>
+      <c r="L29" s="94"/>
       <c r="M29" s="86"/>
       <c r="N29" s="86"/>
       <c r="O29" s="87"/>
       <c r="P29" s="86"/>
       <c r="Q29" s="84"/>
       <c r="R29" s="85"/>
-      <c r="S29" s="86"/>
+      <c r="S29" s="14"/>
       <c r="T29" s="84"/>
-      <c r="U29" s="97"/>
+      <c r="U29" s="98"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="96" t="s">
-        <v>556</v>
-      </c>
-      <c r="B30" s="108" t="s">
-        <v>557</v>
-      </c>
-      <c r="C30" s="103" t="s">
-        <v>691</v>
-      </c>
-      <c r="D30" s="95">
+      <c r="A30" s="78" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="78" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="79" t="s">
+        <v>689</v>
+      </c>
+      <c r="D30" s="80">
         <v>5.0</v>
       </c>
       <c r="E30" s="81" t="s">
         <v>54</v>
       </c>
       <c r="F30" s="81" t="s">
-        <v>692</v>
-      </c>
-      <c r="G30" s="84" t="s">
-        <v>693</v>
+        <v>690</v>
+      </c>
+      <c r="G30" s="112" t="s">
+        <v>691</v>
       </c>
       <c r="H30" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I30" s="85"/>
-      <c r="J30" s="85"/>
+      <c r="I30" s="86"/>
+      <c r="J30" s="86"/>
       <c r="K30" s="6"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
+      <c r="L30" s="86"/>
+      <c r="M30" s="86"/>
+      <c r="N30" s="86"/>
       <c r="O30" s="87"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="85"/>
+      <c r="P30" s="86"/>
+      <c r="Q30" s="84"/>
       <c r="R30" s="85"/>
-      <c r="S30" s="14"/>
-      <c r="T30" s="85"/>
-      <c r="U30" s="97"/>
+      <c r="S30" s="86"/>
+      <c r="T30" s="84"/>
+      <c r="U30" s="98"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="96" t="s">
-        <v>558</v>
-      </c>
-      <c r="B31" s="108" t="s">
-        <v>371</v>
-      </c>
-      <c r="C31" s="103" t="s">
-        <v>694</v>
-      </c>
-      <c r="D31" s="95">
+      <c r="A31" s="97" t="s">
+        <v>556</v>
+      </c>
+      <c r="B31" s="110" t="s">
+        <v>557</v>
+      </c>
+      <c r="C31" s="104" t="s">
+        <v>692</v>
+      </c>
+      <c r="D31" s="96">
         <v>5.0</v>
       </c>
       <c r="E31" s="81" t="s">
         <v>54</v>
       </c>
       <c r="F31" s="81" t="s">
-        <v>695</v>
-      </c>
-      <c r="G31" s="84" t="s">
-        <v>696</v>
+        <v>693</v>
+      </c>
+      <c r="G31" s="112" t="s">
+        <v>694</v>
       </c>
       <c r="H31" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I31" s="84"/>
+      <c r="I31" s="85"/>
       <c r="J31" s="85"/>
       <c r="K31" s="6"/>
       <c r="L31" s="14"/>
@@ -27880,75 +27972,73 @@
       <c r="R31" s="85"/>
       <c r="S31" s="14"/>
       <c r="T31" s="85"/>
-      <c r="U31" s="97"/>
+      <c r="U31" s="98"/>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="96" t="s">
-        <v>559</v>
-      </c>
-      <c r="B32" s="108" t="s">
-        <v>560</v>
-      </c>
-      <c r="C32" s="103" t="s">
+      <c r="A32" s="97" t="s">
+        <v>558</v>
+      </c>
+      <c r="B32" s="110" t="s">
+        <v>371</v>
+      </c>
+      <c r="C32" s="104" t="s">
+        <v>695</v>
+      </c>
+      <c r="D32" s="96">
+        <v>5.0</v>
+      </c>
+      <c r="E32" s="81" t="s">
+        <v>54</v>
+      </c>
+      <c r="F32" s="81" t="s">
+        <v>696</v>
+      </c>
+      <c r="G32" s="112" t="s">
         <v>697</v>
-      </c>
-      <c r="D32" s="95">
-        <v>5.0</v>
-      </c>
-      <c r="E32" s="81">
-        <v>6.0</v>
-      </c>
-      <c r="F32" s="81" t="s">
-        <v>698</v>
-      </c>
-      <c r="G32" s="84" t="s">
-        <v>699</v>
       </c>
       <c r="H32" s="83" t="s">
         <v>599</v>
       </c>
       <c r="I32" s="84"/>
-      <c r="J32" s="86"/>
-      <c r="K32" s="86"/>
-      <c r="L32" s="86"/>
-      <c r="M32" s="104"/>
-      <c r="N32" s="86"/>
-      <c r="O32" s="90"/>
-      <c r="P32" s="86"/>
-      <c r="Q32" s="84"/>
-      <c r="R32" s="86"/>
-      <c r="S32" s="86"/>
-      <c r="T32" s="84"/>
-      <c r="U32" s="97"/>
-    </row>
-    <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="96" t="s">
+      <c r="J32" s="85"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="87"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="85"/>
+      <c r="R32" s="85"/>
+      <c r="S32" s="14"/>
+      <c r="T32" s="85"/>
+      <c r="U32" s="98"/>
+    </row>
+    <row r="33" ht="57.0" customHeight="1">
+      <c r="A33" s="97" t="s">
         <v>565</v>
       </c>
-      <c r="B33" s="108" t="s">
+      <c r="B33" s="110" t="s">
         <v>151</v>
       </c>
-      <c r="C33" s="103" t="s">
-        <v>700</v>
-      </c>
-      <c r="D33" s="95">
+      <c r="C33" s="104" t="s">
+        <v>698</v>
+      </c>
+      <c r="D33" s="96">
         <v>5.0</v>
       </c>
       <c r="E33" s="81" t="s">
         <v>54</v>
       </c>
       <c r="F33" s="81" t="s">
-        <v>701</v>
-      </c>
-      <c r="G33" s="84" t="s">
-        <v>702</v>
+        <v>699</v>
+      </c>
+      <c r="G33" s="112" t="s">
+        <v>700</v>
       </c>
       <c r="H33" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I33" s="84" t="s">
-        <v>703</v>
-      </c>
+      <c r="I33" s="84"/>
       <c r="J33" s="84"/>
       <c r="K33" s="84"/>
       <c r="L33" s="86"/>
@@ -27960,46 +28050,46 @@
       <c r="R33" s="86"/>
       <c r="S33" s="86"/>
       <c r="T33" s="84"/>
-      <c r="U33" s="97"/>
-    </row>
-    <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="96" t="s">
+      <c r="U33" s="98"/>
+    </row>
+    <row r="34" ht="54.75" customHeight="1">
+      <c r="A34" s="97" t="s">
         <v>575</v>
       </c>
-      <c r="B34" s="110" t="s">
+      <c r="B34" s="113" t="s">
         <v>151</v>
       </c>
-      <c r="C34" s="103" t="s">
-        <v>704</v>
-      </c>
-      <c r="D34" s="95">
+      <c r="C34" s="104" t="s">
+        <v>701</v>
+      </c>
+      <c r="D34" s="96">
         <v>3.0</v>
       </c>
       <c r="E34" s="92">
         <v>7.0</v>
       </c>
       <c r="F34" s="92" t="s">
-        <v>705</v>
-      </c>
-      <c r="G34" s="84" t="s">
-        <v>706</v>
+        <v>702</v>
+      </c>
+      <c r="G34" s="112" t="s">
+        <v>703</v>
       </c>
       <c r="H34" s="83" t="s">
         <v>599</v>
       </c>
       <c r="I34" s="84"/>
-      <c r="J34" s="93"/>
+      <c r="J34" s="94"/>
       <c r="K34" s="84"/>
-      <c r="L34" s="93"/>
-      <c r="M34" s="93"/>
+      <c r="L34" s="94"/>
+      <c r="M34" s="94"/>
       <c r="N34" s="86"/>
       <c r="O34" s="90"/>
       <c r="P34" s="86"/>
       <c r="Q34" s="84"/>
       <c r="R34" s="84"/>
-      <c r="S34" s="93"/>
+      <c r="S34" s="94"/>
       <c r="T34" s="85"/>
-      <c r="U34" s="97"/>
+      <c r="U34" s="98"/>
     </row>
     <row r="35" ht="14.25" customHeight="1">
       <c r="A35" s="78" t="s">
@@ -28008,8 +28098,8 @@
       <c r="B35" s="10" t="s">
         <v>373</v>
       </c>
-      <c r="C35" s="103" t="s">
-        <v>707</v>
+      <c r="C35" s="104" t="s">
+        <v>704</v>
       </c>
       <c r="D35" s="80">
         <v>5.0</v>
@@ -28018,115 +28108,115 @@
         <v>54</v>
       </c>
       <c r="F35" s="92" t="s">
-        <v>708</v>
-      </c>
-      <c r="G35" s="93" t="s">
-        <v>709</v>
+        <v>705</v>
+      </c>
+      <c r="G35" s="114" t="s">
+        <v>706</v>
       </c>
       <c r="H35" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I35" s="93"/>
+      <c r="I35" s="94"/>
       <c r="J35" s="88"/>
       <c r="K35" s="88"/>
       <c r="L35" s="88"/>
-      <c r="M35" s="106"/>
-      <c r="N35" s="106"/>
+      <c r="M35" s="108"/>
+      <c r="N35" s="108"/>
       <c r="O35" s="87"/>
       <c r="P35" s="14"/>
       <c r="Q35" s="85"/>
-      <c r="R35" s="106"/>
-      <c r="S35" s="106"/>
+      <c r="R35" s="108"/>
+      <c r="S35" s="108"/>
       <c r="T35" s="84"/>
-      <c r="U35" s="97"/>
+      <c r="U35" s="98"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="96" t="s">
+      <c r="A36" s="97" t="s">
         <v>584</v>
       </c>
-      <c r="B36" s="110" t="s">
+      <c r="B36" s="113" t="s">
         <v>585</v>
       </c>
-      <c r="C36" s="103" t="s">
-        <v>710</v>
-      </c>
-      <c r="D36" s="95">
+      <c r="C36" s="104" t="s">
+        <v>707</v>
+      </c>
+      <c r="D36" s="96">
         <v>5.0</v>
       </c>
       <c r="E36" s="81" t="s">
         <v>54</v>
       </c>
       <c r="F36" s="92" t="s">
-        <v>711</v>
-      </c>
-      <c r="G36" s="93" t="s">
-        <v>712</v>
+        <v>708</v>
+      </c>
+      <c r="G36" s="114" t="s">
+        <v>709</v>
       </c>
       <c r="H36" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I36" s="93"/>
-      <c r="J36" s="106"/>
+      <c r="I36" s="94"/>
+      <c r="J36" s="108"/>
       <c r="K36" s="6"/>
-      <c r="L36" s="106"/>
-      <c r="M36" s="106"/>
-      <c r="N36" s="106"/>
+      <c r="L36" s="108"/>
+      <c r="M36" s="108"/>
+      <c r="N36" s="108"/>
       <c r="O36" s="87"/>
       <c r="P36" s="14"/>
       <c r="Q36" s="85"/>
-      <c r="R36" s="106"/>
-      <c r="S36" s="106"/>
+      <c r="R36" s="108"/>
+      <c r="S36" s="108"/>
       <c r="T36" s="85"/>
-      <c r="U36" s="97"/>
+      <c r="U36" s="98"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="96" t="s">
-        <v>713</v>
-      </c>
-      <c r="B37" s="110" t="s">
+      <c r="A37" s="97" t="s">
+        <v>710</v>
+      </c>
+      <c r="B37" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="C37" s="103" t="s">
-        <v>714</v>
-      </c>
-      <c r="D37" s="95">
+      <c r="C37" s="91" t="s">
+        <v>711</v>
+      </c>
+      <c r="D37" s="96">
         <v>5.0</v>
       </c>
       <c r="E37" s="81" t="s">
         <v>54</v>
       </c>
       <c r="F37" s="92" t="s">
-        <v>715</v>
-      </c>
-      <c r="G37" s="93" t="s">
-        <v>716</v>
+        <v>712</v>
+      </c>
+      <c r="G37" s="115" t="s">
+        <v>713</v>
       </c>
       <c r="H37" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I37" s="106"/>
-      <c r="J37" s="93"/>
+      <c r="I37" s="108"/>
+      <c r="J37" s="94"/>
       <c r="K37" s="6"/>
-      <c r="L37" s="106"/>
-      <c r="M37" s="106"/>
-      <c r="N37" s="106"/>
+      <c r="L37" s="108"/>
+      <c r="M37" s="108"/>
+      <c r="N37" s="108"/>
       <c r="O37" s="87"/>
       <c r="P37" s="14"/>
       <c r="Q37" s="85"/>
-      <c r="R37" s="106"/>
-      <c r="S37" s="106"/>
+      <c r="R37" s="108"/>
+      <c r="S37" s="108"/>
       <c r="T37" s="85"/>
-      <c r="U37" s="97"/>
+      <c r="U37" s="98"/>
     </row>
     <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="107" t="s">
+      <c r="A38" s="109" t="s">
         <v>183</v>
       </c>
       <c r="B38" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="C38" s="103" t="s">
-        <v>717</v>
+      <c r="C38" s="104" t="s">
+        <v>714</v>
       </c>
       <c r="D38" s="87">
         <v>5.0</v>
@@ -28135,15 +28225,15 @@
         <v>54</v>
       </c>
       <c r="F38" s="92" t="s">
-        <v>718</v>
-      </c>
-      <c r="G38" s="93" t="s">
-        <v>719</v>
+        <v>715</v>
+      </c>
+      <c r="G38" s="114" t="s">
+        <v>716</v>
       </c>
       <c r="H38" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I38" s="106"/>
+      <c r="I38" s="108"/>
       <c r="J38" s="85"/>
       <c r="K38" s="6"/>
       <c r="L38" s="14"/>
@@ -28155,29 +28245,29 @@
       <c r="R38" s="85"/>
       <c r="S38" s="14"/>
       <c r="T38" s="85"/>
-      <c r="U38" s="97"/>
+      <c r="U38" s="98"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="108" t="s">
+      <c r="A39" s="110" t="s">
         <v>587</v>
       </c>
-      <c r="B39" s="108" t="s">
-        <v>720</v>
-      </c>
-      <c r="C39" s="111" t="s">
-        <v>721</v>
-      </c>
-      <c r="D39" s="112">
+      <c r="B39" s="110" t="s">
+        <v>717</v>
+      </c>
+      <c r="C39" s="116" t="s">
+        <v>718</v>
+      </c>
+      <c r="D39" s="117">
         <v>5.0</v>
       </c>
       <c r="E39" s="81" t="s">
         <v>54</v>
       </c>
       <c r="F39" s="86" t="s">
-        <v>722</v>
-      </c>
-      <c r="G39" s="84" t="s">
-        <v>723</v>
+        <v>719</v>
+      </c>
+      <c r="G39" s="112" t="s">
+        <v>720</v>
       </c>
       <c r="H39" s="83" t="s">
         <v>599</v>
@@ -28197,30 +28287,30 @@
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="25" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>725</v>
-      </c>
-      <c r="C40" s="113" t="s">
-        <v>726</v>
+        <v>722</v>
+      </c>
+      <c r="C40" s="118" t="s">
+        <v>723</v>
       </c>
       <c r="D40" s="25">
         <v>3.0</v>
       </c>
-      <c r="E40" s="114">
+      <c r="E40" s="119">
         <v>7.0</v>
       </c>
-      <c r="F40" s="114" t="s">
-        <v>727</v>
-      </c>
-      <c r="G40" s="114" t="s">
-        <v>728</v>
+      <c r="F40" s="119" t="s">
+        <v>724</v>
+      </c>
+      <c r="G40" s="120" t="s">
+        <v>725</v>
       </c>
       <c r="H40" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="I40" s="114"/>
+      <c r="I40" s="119"/>
       <c r="J40" s="70"/>
       <c r="K40" s="6"/>
       <c r="L40" s="70"/>
@@ -43466,49 +43556,50 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C2"/>
-    <hyperlink r:id="rId2" ref="C3"/>
-    <hyperlink r:id="rId3" ref="C4"/>
-    <hyperlink r:id="rId4" ref="C5"/>
-    <hyperlink r:id="rId5" ref="C6"/>
-    <hyperlink r:id="rId6" ref="C7"/>
-    <hyperlink r:id="rId7" ref="C8"/>
-    <hyperlink r:id="rId8" ref="C9"/>
-    <hyperlink r:id="rId9" ref="C10"/>
-    <hyperlink r:id="rId10" ref="C11"/>
-    <hyperlink r:id="rId11" ref="C12"/>
-    <hyperlink r:id="rId12" ref="C13"/>
-    <hyperlink r:id="rId13" ref="C14"/>
-    <hyperlink r:id="rId14" ref="C15"/>
-    <hyperlink r:id="rId15" ref="C16"/>
-    <hyperlink r:id="rId16" ref="C17"/>
-    <hyperlink r:id="rId17" ref="C18"/>
-    <hyperlink r:id="rId18" ref="C19"/>
-    <hyperlink r:id="rId19" ref="C20"/>
-    <hyperlink r:id="rId20" ref="C21"/>
-    <hyperlink r:id="rId21" ref="C22"/>
-    <hyperlink r:id="rId22" ref="C23"/>
-    <hyperlink r:id="rId23" ref="C24"/>
-    <hyperlink r:id="rId24" ref="C25"/>
-    <hyperlink r:id="rId25" ref="C26"/>
-    <hyperlink r:id="rId26" ref="C27"/>
-    <hyperlink r:id="rId27" ref="C28"/>
-    <hyperlink r:id="rId28" ref="C29"/>
-    <hyperlink r:id="rId29" ref="C30"/>
-    <hyperlink r:id="rId30" ref="C31"/>
-    <hyperlink r:id="rId31" ref="C32"/>
-    <hyperlink r:id="rId32" ref="C33"/>
-    <hyperlink r:id="rId33" ref="C34"/>
-    <hyperlink r:id="rId34" ref="C35"/>
-    <hyperlink r:id="rId35" ref="C36"/>
-    <hyperlink r:id="rId36" ref="C37"/>
-    <hyperlink r:id="rId37" ref="C38"/>
-    <hyperlink r:id="rId38" ref="C39"/>
-    <hyperlink r:id="rId39" ref="C40"/>
+    <hyperlink r:id="rId2" ref="C2"/>
+    <hyperlink r:id="rId3" ref="C3"/>
+    <hyperlink r:id="rId4" ref="C4"/>
+    <hyperlink r:id="rId5" ref="C5"/>
+    <hyperlink r:id="rId6" ref="C6"/>
+    <hyperlink r:id="rId7" ref="C7"/>
+    <hyperlink r:id="rId8" ref="C8"/>
+    <hyperlink r:id="rId9" ref="C9"/>
+    <hyperlink r:id="rId10" ref="C10"/>
+    <hyperlink r:id="rId11" ref="C11"/>
+    <hyperlink r:id="rId12" ref="C12"/>
+    <hyperlink r:id="rId13" ref="C13"/>
+    <hyperlink r:id="rId14" ref="C14"/>
+    <hyperlink r:id="rId15" ref="C15"/>
+    <hyperlink r:id="rId16" ref="C16"/>
+    <hyperlink r:id="rId17" ref="C17"/>
+    <hyperlink r:id="rId18" ref="C18"/>
+    <hyperlink r:id="rId19" ref="C19"/>
+    <hyperlink r:id="rId20" ref="C20"/>
+    <hyperlink r:id="rId21" ref="C21"/>
+    <hyperlink r:id="rId22" ref="C22"/>
+    <hyperlink r:id="rId23" ref="C23"/>
+    <hyperlink r:id="rId24" ref="C24"/>
+    <hyperlink r:id="rId25" ref="C25"/>
+    <hyperlink r:id="rId26" ref="C26"/>
+    <hyperlink r:id="rId27" ref="C27"/>
+    <hyperlink r:id="rId28" ref="C28"/>
+    <hyperlink r:id="rId29" ref="C29"/>
+    <hyperlink r:id="rId30" ref="C30"/>
+    <hyperlink r:id="rId31" ref="C31"/>
+    <hyperlink r:id="rId32" ref="C32"/>
+    <hyperlink r:id="rId33" ref="C33"/>
+    <hyperlink r:id="rId34" ref="C34"/>
+    <hyperlink r:id="rId35" ref="C35"/>
+    <hyperlink r:id="rId36" ref="C36"/>
+    <hyperlink r:id="rId37" ref="C37"/>
+    <hyperlink r:id="rId38" ref="C38"/>
+    <hyperlink r:id="rId39" ref="C39"/>
+    <hyperlink r:id="rId40" ref="C40"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId40"/>
+  <drawing r:id="rId41"/>
+  <legacyDrawing r:id="rId42"/>
 </worksheet>
 </file>
</xml_diff>